<commit_message>
-Creating SIQ template -Correcting typo in project plan
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4EE610-6B71-4357-A312-90720C36FE90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,9 +14,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Req_id</t>
+  </si>
+  <si>
+    <t>SIQ_id</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Proposed Answer</t>
+  </si>
+  <si>
+    <t>Question Submit Date</t>
+  </si>
+  <si>
+    <t>Expected Response Date</t>
+  </si>
+  <si>
+    <t>Return Answer Date</t>
+  </si>
+  <si>
+    <t>Answer Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Interactive Questionaire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Which Document </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +59,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -40,18 +120,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -131,9 +271,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,6 +323,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -341,13 +515,387 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I30" xr:uid="{2D8A5949-CD00-4543-B03C-6E009F079359}">
+      <formula1>"Fully answered, No statisfing answer"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Answering from SIQ004 to SIQ016 Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="172"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
   <si>
     <t>SIQ_id</t>
   </si>
@@ -191,13 +191,81 @@
   </si>
   <si>
     <t>St startup mode2 When all LEDs are activated, is it turned of in sequence also or at the same time ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 ms </t>
+  </si>
+  <si>
+    <t>No, the sequenc will be as follows:
+All leds OFF except L6 is ON
+All leds OFF except L5 is ON
+All leds OFF except L4 is ON
+All leds OFF except L3 is ON
+All leds OFF except L2 is ON
+All leds OFF except L1 is ON
+All leds OFF except R1 is ON
+All leds OFF except R2 is ON
+All leds OFF except R3 is ON
+All leds OFF except R4 is ON
+All leds OFF except R5 is ON
+All leds OFF except R6 is ON
+Then
+All leds OFF
+Then
+All leds OFF except R6 is ON
+All leds OFF except R5 is ON
+All leds OFF except R4 is ON
+All leds OFF except R3 is ON
+All leds OFF except R2 is ON
+All leds OFF except R1 is ON
+All leds OFF except L1 is ON
+All leds OFF except L2 is ON
+All leds OFF except L3 is ON
+All leds OFF except L4 is ON
+All leds OFF except L5 is ON
+All leds OFF except L6 is ON
+Then
+All leds OFF
+Then
+All leds including Tail leds are ON
+Then
+All ldes including Tail leds are OFF</t>
+  </si>
+  <si>
+    <t>Explained in details in SIQ005</t>
+  </si>
+  <si>
+    <t>200ms</t>
+  </si>
+  <si>
+    <t>300ms</t>
+  </si>
+  <si>
+    <t>Repeated for just one more time</t>
+  </si>
+  <si>
+    <t>All leds OFF except R1,L1 are ON
+All leds OFF except R2,L2 are ON
+All leds OFF except R3,L3 are ON
+All leds OFF except R4,L4 are ON
+All leds OFF except R5,L5 are ON
+All leds OFF except R6,L6 are ON</t>
+  </si>
+  <si>
+    <t>Yes, I just need a high level or low level to decide the mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No TI function has 2 separate switches, one for right TI and another for left TI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Leds will be deactivated at the same time </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,7 +430,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -405,6 +473,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -468,7 +539,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,10 +571,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,7 +605,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,14 +780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" style="9" customWidth="1"/>
     <col min="2" max="2" width="41" style="9" customWidth="1"/>
@@ -733,7 +802,7 @@
     <col min="11" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="14" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="14" customFormat="1" ht="55.5" customHeight="1">
       <c r="A1" s="12"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -742,7 +811,7 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="42" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -806,7 +875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="61.5" thickTop="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -838,7 +907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="61.5" thickTop="1" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -870,14 +939,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="46.5" thickTop="1" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="8">
         <v>43892</v>
@@ -885,7 +956,9 @@
       <c r="F6" s="8">
         <v>43892</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="8">
+        <v>43892</v>
+      </c>
       <c r="H6" s="3" t="s">
         <v>17</v>
       </c>
@@ -896,14 +969,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="409.6" thickTop="1" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="8">
         <v>43892</v>
@@ -911,7 +986,9 @@
       <c r="F7" s="8">
         <v>43892</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="8">
+        <v>43892</v>
+      </c>
       <c r="H7" s="3" t="s">
         <v>17</v>
       </c>
@@ -922,14 +999,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="61.5" thickTop="1" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
@@ -939,7 +1018,9 @@
       <c r="F8" s="8">
         <v>43892</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="8">
+        <v>43893</v>
+      </c>
       <c r="H8" s="3" t="s">
         <v>17</v>
       </c>
@@ -950,14 +1031,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="46.5" thickTop="1" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="8">
         <v>43892</v>
@@ -965,7 +1048,9 @@
       <c r="F9" s="8">
         <v>43892</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8">
+        <v>43892</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>17</v>
       </c>
@@ -976,14 +1061,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="8">
         <v>43892</v>
@@ -991,7 +1078,9 @@
       <c r="F10" s="8">
         <v>43892</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8">
+        <v>43893</v>
+      </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1002,14 +1091,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="46.5" thickTop="1" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="8">
         <v>43892</v>
@@ -1017,7 +1108,9 @@
       <c r="F11" s="8">
         <v>43892</v>
       </c>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8">
+        <v>43894</v>
+      </c>
       <c r="H11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1028,14 +1121,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="91.5" thickTop="1" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="8">
         <v>43892</v>
@@ -1043,7 +1138,9 @@
       <c r="F12" s="8">
         <v>43892</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="8">
+        <v>43895</v>
+      </c>
       <c r="H12" s="3" t="s">
         <v>17</v>
       </c>
@@ -1054,14 +1151,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="8">
         <v>43892</v>
@@ -1069,7 +1168,9 @@
       <c r="F13" s="8">
         <v>43892</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="8">
+        <v>43896</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1080,14 +1181,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D14" s="3"/>
       <c r="E14" s="8">
         <v>43892</v>
@@ -1095,7 +1198,9 @@
       <c r="F14" s="8">
         <v>43892</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="8">
+        <v>43897</v>
+      </c>
       <c r="H14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1106,14 +1211,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="61.5" thickTop="1" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="D15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1123,7 +1230,9 @@
       <c r="F15" s="8">
         <v>43892</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="8">
+        <v>43898</v>
+      </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1134,14 +1243,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="46.5" thickTop="1" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="D16" s="3" t="s">
         <v>57</v>
       </c>
@@ -1151,7 +1262,9 @@
       <c r="F16" s="8">
         <v>43892</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="8">
+        <v>43899</v>
+      </c>
       <c r="H16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1162,14 +1275,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="8">
         <v>43892</v>
@@ -1177,7 +1292,9 @@
       <c r="F17" s="8">
         <v>43892</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="8">
+        <v>43900</v>
+      </c>
       <c r="H17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1188,23 +1305,33 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="E18" s="8">
+        <v>43892</v>
+      </c>
+      <c r="F18" s="8">
+        <v>43892</v>
+      </c>
+      <c r="G18" s="8">
+        <v>43901</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I18" s="7"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1216,7 +1343,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1228,7 +1355,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1240,7 +1367,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1252,7 +1379,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1264,7 +1391,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1276,7 +1403,7 @@
       <c r="I24" s="7"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1288,7 +1415,7 @@
       <c r="I25" s="7"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1300,7 +1427,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1312,7 +1439,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1324,7 +1451,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1336,7 +1463,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1348,7 +1475,7 @@
       <c r="I30" s="7"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1360,7 +1487,7 @@
       <c r="I31" s="7"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1372,7 +1499,7 @@
       <c r="I32" s="7"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1384,7 +1511,7 @@
       <c r="I33" s="7"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1396,7 +1523,7 @@
       <c r="I34" s="7"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1408,7 +1535,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" thickTop="1">
       <c r="I36" s="10"/>
     </row>
   </sheetData>

</xml_diff>